<commit_message>
Modify javadoc and performance result
</commit_message>
<xml_diff>
--- a/sorm4j-jmh/public/result/jmh-results.xlsx
+++ b/sorm4j-jmh/public/result/jmh-results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\home\ws\sorm4j\sorm4j-jmh\public\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC1846E-2F1F-4D45-90D5-D6C2297D9DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3839FA-69FD-42C9-B2F7-142D29E22A90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{9D1FDE6F-6CE7-48B5-8FE2-8070845FD5C3}"/>
   </bookViews>
@@ -23,15 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -408,10 +399,10 @@
                   <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.9</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3983,22 +3974,22 @@
                   <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.2</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.2</c:v>
+                  <c:v>42.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4621,22 +4612,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3343</c:v>
+                  <c:v>3405</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3281</c:v>
+                  <c:v>3091</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4046</c:v>
+                  <c:v>3878</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5196</c:v>
+                  <c:v>5128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14273</c:v>
+                  <c:v>14123</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10273</c:v>
+                  <c:v>10083</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4940,16 +4931,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>21405</c:v>
+                  <c:v>21135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22067</c:v>
+                  <c:v>21259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42954</c:v>
+                  <c:v>41126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37186</c:v>
+                  <c:v>37644</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18390,7 +18381,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0B099F85-E6F2-4D11-85FB-BA203DF3B02D}" name="テーブル13456" displayName="テーブル13456" ref="A1:E22" totalsRowShown="0">
   <autoFilter ref="A1:E22" xr:uid="{373D6382-5638-4456-A6E1-BFB64FFC50EB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+  <sortState ref="A2:E22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="5">
@@ -18409,7 +18400,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6482DFFA-EEF8-42ED-B03C-076350F6DC81}" name="テーブル1345" displayName="テーブル1345" ref="A1:E23" totalsRowShown="0">
   <autoFilter ref="A1:E23" xr:uid="{373D6382-5638-4456-A6E1-BFB64FFC50EB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+  <sortState ref="A2:E23">
     <sortCondition ref="B1:B23"/>
   </sortState>
   <tableColumns count="5">
@@ -18428,7 +18419,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{374BC028-046E-41DD-BDE2-60820EC6950B}" name="テーブル134" displayName="テーブル134" ref="A1:E23" totalsRowShown="0">
   <autoFilter ref="A1:E23" xr:uid="{373D6382-5638-4456-A6E1-BFB64FFC50EB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+  <sortState ref="A2:E23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="5">
@@ -18447,7 +18438,7 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FF856B7-87CB-42F1-B811-6D2A4CA1C1D6}" name="テーブル13" displayName="テーブル13" ref="A1:E23" totalsRowShown="0">
   <autoFilter ref="A1:E23" xr:uid="{373D6382-5638-4456-A6E1-BFB64FFC50EB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+  <sortState ref="A2:E23">
     <sortCondition ref="C1:C23"/>
   </sortState>
   <tableColumns count="5">
@@ -18466,7 +18457,7 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3DFB630-8B09-4E21-9911-22AE76885298}" name="テーブル1" displayName="テーブル1" ref="A1:E23" totalsRowShown="0">
   <autoFilter ref="A1:E23" xr:uid="{373D6382-5638-4456-A6E1-BFB64FFC50EB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+  <sortState ref="A2:E23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="5">
@@ -18781,8 +18772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5D3ACD-9F98-4EB6-8D76-E5E3AF866B50}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -18845,10 +18836,10 @@
         <v>handCodedInsert</v>
       </c>
       <c r="D2">
-        <v>5.1718229999999998</v>
+        <v>5.2318110000000004</v>
       </c>
       <c r="E2">
-        <v>0.13993</v>
+        <v>0.124401</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
@@ -18863,11 +18854,11 @@
       </c>
       <c r="M2">
         <f>ROUND(VLOOKUP(CONCATENATE($H2,M$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>3343</v>
+        <v>3405</v>
       </c>
       <c r="O2">
         <f>ROUND(VLOOKUP(CONCATENATE($H2,O$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>21405</v>
+        <v>21135</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
@@ -18882,21 +18873,21 @@
         <v>handCodedMultiRowInsert</v>
       </c>
       <c r="D3">
-        <v>21404.635849999999</v>
+        <v>21134.842909999999</v>
       </c>
       <c r="E3">
-        <v>1732.855644</v>
+        <v>1379.4680089999999</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H3,I$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J8" si="0">"(" &amp;ROUND((I3-I$2)/I$2*100,0)&amp;"% slower)"</f>
-        <v>(7% slower)</v>
+        <v>(2% slower)</v>
       </c>
       <c r="K3" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H3,K$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
@@ -18908,19 +18899,19 @@
       </c>
       <c r="M3">
         <f>ROUND(VLOOKUP(CONCATENATE($H3,M$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>3281</v>
+        <v>3091</v>
       </c>
       <c r="N3" t="str">
         <f>"(" &amp;ROUND((M3-M$2)/M$2*100,0)&amp;"% slower)"</f>
-        <v>(-2% slower)</v>
+        <v>(-9% slower)</v>
       </c>
       <c r="O3">
         <f>ROUND(VLOOKUP(CONCATENATE($H3,O$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>22067</v>
+        <v>21259</v>
       </c>
       <c r="P3" t="str">
         <f>"(" &amp;ROUND((O3-O$2)/O$2*100,0)&amp;"% slower)"</f>
-        <v>(3% slower)</v>
+        <v>(1% slower)</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
@@ -18935,45 +18926,45 @@
         <v>handCodedReadAll</v>
       </c>
       <c r="D4">
-        <v>3342.5736040000002</v>
+        <v>3404.8455260000001</v>
       </c>
       <c r="E4">
-        <v>72.758968999999993</v>
+        <v>94.134073000000001</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H4,I$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>(55% slower)</v>
+        <v>(50% slower)</v>
       </c>
       <c r="K4" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H4,K$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>9.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="L4" t="str">
         <f>"(" &amp;ROUND((K4-K$2)/K$2*100,0)&amp;"% slower)"</f>
-        <v>(85% slower)</v>
+        <v>(79% slower)</v>
       </c>
       <c r="M4">
         <f>ROUND(VLOOKUP(CONCATENATE($H4,M$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>4046</v>
+        <v>3878</v>
       </c>
       <c r="N4" t="str">
         <f>"(" &amp;ROUND((M4-M$2)/M$2*100,0)&amp;"% slower)"</f>
-        <v>(21% slower)</v>
+        <v>(14% slower)</v>
       </c>
       <c r="O4">
         <f>ROUND(VLOOKUP(CONCATENATE($H4,O$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>42954</v>
+        <v>41126</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" ref="P4:P5" si="1">"(" &amp;ROUND((O4-O$2)/O$2*100,0)&amp;"% slower)"</f>
-        <v>(101% slower)</v>
+        <v>(95% slower)</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
@@ -18988,45 +18979,45 @@
         <v>handCodedReadOne</v>
       </c>
       <c r="D5">
-        <v>4.229698</v>
+        <v>4.1886109999999999</v>
       </c>
       <c r="E5">
-        <v>4.2298000000000002E-2</v>
+        <v>3.0286E-2</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H5,I$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>16.2</v>
+        <v>16.5</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>(286% slower)</v>
+        <v>(293% slower)</v>
       </c>
       <c r="K5" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H5,K$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="L5" t="str">
         <f>"(" &amp;ROUND((K5-K$2)/K$2*100,0)&amp;"% slower)"</f>
-        <v>(129% slower)</v>
+        <v>(133% slower)</v>
       </c>
       <c r="M5">
         <f>ROUND(VLOOKUP(CONCATENATE($H5,M$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>5196</v>
+        <v>5128</v>
       </c>
       <c r="N5" t="str">
         <f>"(" &amp;ROUND((M5-M$2)/M$2*100,0)&amp;"% slower)"</f>
-        <v>(55% slower)</v>
+        <v>(51% slower)</v>
       </c>
       <c r="O5">
         <f>ROUND(VLOOKUP(CONCATENATE($H5,O$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>37186</v>
+        <v>37644</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="1"/>
-        <v>(74% slower)</v>
+        <v>(78% slower)</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
@@ -19041,30 +19032,30 @@
         <v>jDBIInsert</v>
       </c>
       <c r="D6">
-        <v>11.882982999999999</v>
+        <v>12.078761999999999</v>
       </c>
       <c r="E6">
-        <v>0.50490599999999997</v>
+        <v>0.35935299999999998</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H6,I$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>44.2</v>
+        <v>42.9</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>(952% slower)</v>
+        <v>(921% slower)</v>
       </c>
       <c r="K6" s="2"/>
       <c r="M6">
         <f>ROUND(VLOOKUP(CONCATENATE($H6,M$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>14273</v>
+        <v>14123</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" ref="N6:N7" si="2">"(" &amp;ROUND((M6-M$2)/M$2*100,0)&amp;"% slower)"</f>
-        <v>(327% slower)</v>
+        <v>(315% slower)</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.4">
@@ -19079,30 +19070,30 @@
         <v>jDBIMultiRowInsert</v>
       </c>
       <c r="D7">
-        <v>37185.790130000001</v>
+        <v>37644.10643</v>
       </c>
       <c r="E7">
-        <v>1272.00935</v>
+        <v>1376.000933</v>
       </c>
       <c r="H7" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H7,I$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>(138% slower)</v>
+        <v>(129% slower)</v>
       </c>
       <c r="K7" s="2"/>
       <c r="M7">
         <f>ROUND(VLOOKUP(CONCATENATE($H7,M$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),0)</f>
-        <v>10273</v>
+        <v>10083</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="2"/>
-        <v>(207% slower)</v>
+        <v>(196% slower)</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.4">
@@ -19117,21 +19108,21 @@
         <v>jDBIReadAll</v>
       </c>
       <c r="D8">
-        <v>5196.333181</v>
+        <v>5128.2265619999998</v>
       </c>
       <c r="E8">
-        <v>30.318816999999999</v>
+        <v>171.65794099999999</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="2">
         <f>ROUND(VLOOKUP(CONCATENATE($H8,I$1),テーブル13456[[#All],[lib and task]:[error]],2,FALSE),1)</f>
-        <v>9.1</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>(117% slower)</v>
+        <v>(107% slower)</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -19147,10 +19138,10 @@
         <v>jDBIReadOne</v>
       </c>
       <c r="D9">
-        <v>16.210146999999999</v>
+        <v>16.463118999999999</v>
       </c>
       <c r="E9">
-        <v>0.75587099999999996</v>
+        <v>0.68632099999999996</v>
       </c>
       <c r="I9" s="2"/>
       <c r="K9" s="2"/>
@@ -19167,10 +19158,10 @@
         <v>jOOQReadAll</v>
       </c>
       <c r="D10">
-        <v>14272.711869999999</v>
+        <v>14123.416649999999</v>
       </c>
       <c r="E10">
-        <v>379.23082399999998</v>
+        <v>210.31562700000001</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.4">
@@ -19185,10 +19176,10 @@
         <v>jOOQReadOne</v>
       </c>
       <c r="D11">
-        <v>44.203670000000002</v>
+        <v>42.852682000000001</v>
       </c>
       <c r="E11">
-        <v>0.74849699999999997</v>
+        <v>0.83155199999999996</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.4">
@@ -19203,10 +19194,10 @@
         <v>myBatisReadAll</v>
       </c>
       <c r="D12">
-        <v>10272.620269999999</v>
+        <v>10083.1387</v>
       </c>
       <c r="E12">
-        <v>278.43811299999999</v>
+        <v>235.503016</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
@@ -19221,10 +19212,10 @@
         <v>myBatisReadOne</v>
       </c>
       <c r="D13">
-        <v>10.005481</v>
+        <v>9.6076130000000006</v>
       </c>
       <c r="E13">
-        <v>0.336588</v>
+        <v>0.18263699999999999</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
@@ -19239,10 +19230,10 @@
         <v>sormInsert</v>
       </c>
       <c r="D14">
-        <v>5.7429899999999998</v>
+        <v>5.7073499999999999</v>
       </c>
       <c r="E14">
-        <v>0.14307500000000001</v>
+        <v>0.18166499999999999</v>
       </c>
       <c r="H14" t="s">
         <v>16</v>
@@ -19272,10 +19263,10 @@
         <v>sormMultiRowInsert</v>
       </c>
       <c r="D15">
-        <v>22067.419320000001</v>
+        <v>21259.28384</v>
       </c>
       <c r="E15">
-        <v>1479.7603799999999</v>
+        <v>1491.681773</v>
       </c>
       <c r="H15" t="s">
         <v>25</v>
@@ -19290,11 +19281,11 @@
       </c>
       <c r="K15" t="str">
         <f>_xlfn.CONCAT(M2," ",N2)</f>
-        <v xml:space="preserve">3343 </v>
+        <v xml:space="preserve">3405 </v>
       </c>
       <c r="L15" t="str">
         <f>_xlfn.CONCAT(O2," ",P2)</f>
-        <v xml:space="preserve">21405 </v>
+        <v xml:space="preserve">21135 </v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.4">
@@ -19309,17 +19300,17 @@
         <v>sormReadAll</v>
       </c>
       <c r="D16">
-        <v>3280.6523379999999</v>
+        <v>3091.2804299999998</v>
       </c>
       <c r="E16">
-        <v>267.41111100000001</v>
+        <v>57.027994999999997</v>
       </c>
       <c r="H16" t="s">
         <v>30</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ref="I16:I21" si="3">_xlfn.CONCAT(TEXT(I3,".0")," ",J3)</f>
-        <v>4.5 (7% slower)</v>
+        <v>4.3 (2% slower)</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" ref="J16:J18" si="4">_xlfn.CONCAT(TEXT(K3,".0")," ",L3)</f>
@@ -19327,11 +19318,11 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" ref="K16:K20" si="5">_xlfn.CONCAT(M3," ",N3)</f>
-        <v>3281 (-2% slower)</v>
+        <v>3091 (-9% slower)</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ref="L16:L18" si="6">_xlfn.CONCAT(O3," ",P3)</f>
-        <v>22067 (3% slower)</v>
+        <v>21259 (1% slower)</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
@@ -19346,29 +19337,29 @@
         <v>sormReadOne</v>
       </c>
       <c r="D17">
-        <v>4.4757490000000004</v>
+        <v>4.281161</v>
       </c>
       <c r="E17">
-        <v>0.14319100000000001</v>
+        <v>8.5916000000000006E-2</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="3"/>
-        <v>6.5 (55% slower)</v>
+        <v>6.3 (50% slower)</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="4"/>
-        <v>9.6 (85% slower)</v>
+        <v>9.3 (79% slower)</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="5"/>
-        <v>4046 (21% slower)</v>
+        <v>3878 (14% slower)</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="6"/>
-        <v>42954 (101% slower)</v>
+        <v>41126 (95% slower)</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
@@ -19383,29 +19374,29 @@
         <v>springJdbcTemplateReadOne</v>
       </c>
       <c r="D18">
-        <v>9.0969119999999997</v>
+        <v>8.7179169999999999</v>
       </c>
       <c r="E18">
-        <v>0.29468100000000003</v>
+        <v>6.0080000000000001E-2</v>
       </c>
       <c r="H18" t="s">
         <v>27</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="3"/>
-        <v>16.2 (286% slower)</v>
+        <v>16.5 (293% slower)</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="4"/>
-        <v>11.9 (129% slower)</v>
+        <v>12.1 (133% slower)</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="5"/>
-        <v>5196 (55% slower)</v>
+        <v>5128 (51% slower)</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="6"/>
-        <v>37186 (74% slower)</v>
+        <v>37644 (78% slower)</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
@@ -19420,17 +19411,17 @@
         <v>sql2oInsert</v>
       </c>
       <c r="D19">
-        <v>9.5540450000000003</v>
+        <v>9.3036969999999997</v>
       </c>
       <c r="E19">
-        <v>0.15320400000000001</v>
+        <v>0.26167200000000002</v>
       </c>
       <c r="H19" t="s">
         <v>21</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="3"/>
-        <v>44.2 (952% slower)</v>
+        <v>42.9 (921% slower)</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" ref="J19:J22" si="7">_xlfn.CONCAT(K6," ",L6)</f>
@@ -19438,7 +19429,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="5"/>
-        <v>14273 (327% slower)</v>
+        <v>14123 (315% slower)</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
@@ -19453,17 +19444,17 @@
         <v>sql2oMultiRowInsert</v>
       </c>
       <c r="D20">
-        <v>42954.329960000003</v>
+        <v>41125.664320000003</v>
       </c>
       <c r="E20">
-        <v>1663.573993</v>
+        <v>815.67624599999999</v>
       </c>
       <c r="H20" t="s">
         <v>22</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="3"/>
-        <v>10.0 (138% slower)</v>
+        <v>9.6 (129% slower)</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="7"/>
@@ -19471,7 +19462,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="5"/>
-        <v>10273 (207% slower)</v>
+        <v>10083 (196% slower)</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
@@ -19486,17 +19477,17 @@
         <v>sql2oReadAll</v>
       </c>
       <c r="D21">
-        <v>4046.4365509999998</v>
+        <v>3877.7730769999998</v>
       </c>
       <c r="E21">
-        <v>81.696809000000002</v>
+        <v>178.28181900000001</v>
       </c>
       <c r="H21" t="s">
         <v>31</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="3"/>
-        <v>9.1 (117% slower)</v>
+        <v>8.7 (107% slower)</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="7"/>
@@ -19515,10 +19506,10 @@
         <v>sql2oReadOne</v>
       </c>
       <c r="D22">
-        <v>6.4854649999999996</v>
+        <v>6.3018190000000001</v>
       </c>
       <c r="E22">
-        <v>0.12770300000000001</v>
+        <v>0.12196899999999999</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="7"/>
@@ -19582,11 +19573,11 @@
       </c>
       <c r="K29">
         <f>M2</f>
-        <v>3343</v>
+        <v>3405</v>
       </c>
       <c r="L29">
         <f>O2</f>
-        <v>21405</v>
+        <v>21135</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
@@ -19598,7 +19589,7 @@
       </c>
       <c r="I30" s="2">
         <f t="shared" ref="I30:I35" si="8">I3</f>
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" ref="J30:J35" si="9">K3</f>
@@ -19606,11 +19597,11 @@
       </c>
       <c r="K30">
         <f t="shared" ref="K30:K35" si="10">M3</f>
-        <v>3281</v>
+        <v>3091</v>
       </c>
       <c r="L30">
         <f t="shared" ref="L30:L35" si="11">O3</f>
-        <v>22067</v>
+        <v>21259</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
@@ -19622,19 +19613,19 @@
       </c>
       <c r="I31" s="2">
         <f t="shared" si="8"/>
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="9"/>
-        <v>9.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="K31">
         <f t="shared" si="10"/>
-        <v>4046</v>
+        <v>3878</v>
       </c>
       <c r="L31">
         <f t="shared" si="11"/>
-        <v>42954</v>
+        <v>41126</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
@@ -19646,19 +19637,19 @@
       </c>
       <c r="I32" s="2">
         <f t="shared" si="8"/>
-        <v>16.2</v>
+        <v>16.5</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="9"/>
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="K32">
         <f t="shared" si="10"/>
-        <v>5196</v>
+        <v>5128</v>
       </c>
       <c r="L32">
         <f t="shared" si="11"/>
-        <v>37186</v>
+        <v>37644</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.4">
@@ -19670,7 +19661,7 @@
       </c>
       <c r="I33" s="2">
         <f t="shared" si="8"/>
-        <v>44.2</v>
+        <v>42.9</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" si="9"/>
@@ -19678,7 +19669,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="10"/>
-        <v>14273</v>
+        <v>14123</v>
       </c>
       <c r="L33">
         <f t="shared" si="11"/>
@@ -19691,7 +19682,7 @@
       </c>
       <c r="I34" s="2">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" si="9"/>
@@ -19699,7 +19690,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="10"/>
-        <v>10273</v>
+        <v>10083</v>
       </c>
       <c r="L34">
         <f t="shared" si="11"/>
@@ -19712,7 +19703,7 @@
       </c>
       <c r="I35" s="2">
         <f t="shared" si="8"/>
-        <v>9.1</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" si="9"/>

</xml_diff>